<commit_message>
Comparing the assessment methods. Including a long form version of BSM
</commit_message>
<xml_diff>
--- a/Compile fair trial Cod.xlsx
+++ b/Compile fair trial Cod.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>r</t>
   </si>
@@ -38,9 +38,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>k.sd</t>
-  </si>
-  <si>
     <t>k.low</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>q</t>
   </si>
   <si>
-    <t>q.sd</t>
-  </si>
-  <si>
     <t>Alpha/Obs Error</t>
   </si>
   <si>
@@ -123,6 +117,33 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>q.low</t>
+  </si>
+  <si>
+    <t>q.high</t>
+  </si>
+  <si>
+    <t>log.q</t>
+  </si>
+  <si>
+    <t>log.q.sd</t>
+  </si>
+  <si>
+    <t>Mean 5Yr  Catch</t>
+  </si>
+  <si>
+    <t>Mean 5Yr  CPUE</t>
+  </si>
+  <si>
+    <t>log.k.sd</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>q not set up as prior as not using CPUE</t>
   </si>
 </sst>
 </file>
@@ -138,12 +159,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,8 +185,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,110 +468,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="26" max="26" width="15" customWidth="1"/>
+    <col min="5" max="7" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" customWidth="1"/>
+    <col min="31" max="31" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="D2">
         <v>19809</v>
@@ -551,64 +600,84 @@
       <c r="E2">
         <v>2237</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
+      <c r="F2">
+        <v>5.1459999999999999</v>
+      </c>
+      <c r="G2">
+        <v>2.4750000000000002E-3</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
         <v>0.2</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.8</v>
       </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
       <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2">
-        <v>24761</v>
-      </c>
-      <c r="O2">
-        <v>396180</v>
-      </c>
-      <c r="P2" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2">
+        <v>20700</v>
       </c>
       <c r="Q2">
+        <v>331700</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2">
         <v>0.2</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>0.6</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>0.01</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>0.4</v>
       </c>
-      <c r="U2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" t="s">
-        <v>31</v>
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="1">
+        <f>(0.5 * 0.4 *G2)/F2</f>
+        <v>9.6191216478818528E-5</v>
+      </c>
+      <c r="Z2" s="1">
+        <f>(0.8 *G2)/F2</f>
+        <v>3.8476486591527411E-4</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AF2" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>19809</v>
@@ -617,74 +686,120 @@
         <v>2237</v>
       </c>
       <c r="F3">
+        <v>5.1459999999999999</v>
+      </c>
+      <c r="G3">
+        <v>2.4750000000000002E-3</v>
+      </c>
+      <c r="H3">
         <v>0.5</v>
       </c>
-      <c r="G3">
-        <f>LOG(F3)</f>
+      <c r="I3">
+        <f>LOG(H3)</f>
         <v>-0.3010299956639812</v>
       </c>
-      <c r="H3">
-        <f>ABS(G3-(LOG(0.2))/2)</f>
+      <c r="J3">
+        <f>ABS(I3-(LOG(0.2))/2)</f>
         <v>4.8455006504028175E-2</v>
       </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3">
-        <f>(N2+O2)/2</f>
-        <v>210470.5</v>
-      </c>
-      <c r="L3">
-        <f>LOG(K3)</f>
-        <v>5.3231912327843665</v>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
       </c>
       <c r="M3">
-        <f>(L3-(LOG(N2)))/4</f>
-        <v>0.23235576315640527</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
+        <f>(P2+Q2)/2</f>
+        <v>176200</v>
+      </c>
+      <c r="N3">
+        <f>LOG(M3)</f>
+        <v>5.2460059040760294</v>
+      </c>
+      <c r="O3">
+        <f>(N3-(LOG(P2)))/4</f>
+        <v>0.23250888965477801</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="W3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1">
+        <f>(Y2+Z2)/2</f>
+        <v>2.4047804119704631E-4</v>
+      </c>
+      <c r="AB3" s="1">
+        <f>LOG(AA3)</f>
+        <v>-3.6189245742687213</v>
+      </c>
+      <c r="AC3" s="1">
+        <f>(AB3-(LOG(Y2)))/4</f>
+        <v>9.9485002168009373E-2</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>19809</v>
       </c>
       <c r="E4">
         <v>2237</v>
+      </c>
+      <c r="F4">
+        <v>5.1459999999999999</v>
+      </c>
+      <c r="G4">
+        <v>2.4750000000000002E-3</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1">
+        <f>(Y2+Z2)/2</f>
+        <v>2.4047804119704631E-4</v>
+      </c>
+      <c r="AB4" s="1">
+        <f>LOG(AA4)</f>
+        <v>-3.6189245742687213</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>(AB4-(LOG(Y2)))/4</f>
+        <v>9.9485002168009373E-2</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>